<commit_message>
Se anexan los documentos word y ppt
</commit_message>
<xml_diff>
--- a/01_PruebasManales/01_Inventario-pruebas-exploratorias.xlsx
+++ b/01_PruebasManales/01_Inventario-pruebas-exploratorias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semana8\tallersemana8\01_PruebasManales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88243A2F-5B5D-4046-9E3A-9790738D3A63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D172ABE1-35FB-48B7-AD38-7493399ABB0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="608" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="608" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Funcionalidades" sheetId="5" r:id="rId1"/>
@@ -1336,6 +1336,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1350,9 +1353,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE138453-A6BA-4EC9-A11F-EFF024DA9C5C}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1777,13 +1777,13 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -1796,30 +1796,30 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="2:6" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -1829,13 +1829,13 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="2:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -2083,13 +2083,13 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="2:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2111,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2139,17 +2139,17 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -2166,40 +2166,40 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="2:10" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2219,17 +2219,17 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -2911,17 +2911,17 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>